<commit_message>
Tara Ocean Pangea sample datasets
</commit_message>
<xml_diff>
--- a/Tara_Oceans/AHX/ontologies/sample_NCBI.xlsx
+++ b/Tara_Oceans/AHX/ontologies/sample_NCBI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aponsero/Documents/UA_POSTDOC/projects/Planet_Microbe/Planet_Microbe_data/in_progress/Tara_Oceans/AHX/ontologies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7E0C4C-22BF-A044-B1C7-93EAF09FF4DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384E0FF1-88C1-EE4B-9217-6DA8D37FBB43}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="14000" windowHeight="14180" xr2:uid="{C017D531-B4CD-6B4D-AB3C-059A3D47570B}"/>
   </bookViews>
@@ -32,9 +32,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="59">
   <si>
-    <t>Alias</t>
-  </si>
-  <si>
     <t>BioSample</t>
   </si>
   <si>
@@ -207,6 +204,9 @@
   </si>
   <si>
     <t>https://www.ncbi.nlm.nih.gov/bioproject/213098</t>
+  </si>
+  <si>
+    <t>SampleID_Tara</t>
   </si>
 </sst>
 </file>
@@ -567,392 +567,392 @@
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>42</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>43</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>44</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>45</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>46</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>47</v>
-      </c>
-      <c r="K1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="J2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>